<commit_message>
attack data for 10/24 -janae
</commit_message>
<xml_diff>
--- a/honeypot_data_sheets/attacker_reports_20251024.xlsx
+++ b/honeypot_data_sheets/attacker_reports_20251024.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>server1_1761310366.txt</t>
+          <t>server1_1761356704.txt</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -446,17 +446,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>114.218.80.105</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-10-24 08:53:31.192</t>
+          <t>2025-10-24 21:53:13.653</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-10-24 08:53:31.683</t>
+          <t>2025-10-24 21:53:18.784</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -471,17 +471,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ls &amp;&amp; date &amp;&amp; echo hi &amp;&amp; ls * &amp;&amp; whoami &amp;&amp; who</t>
+          <t>/ip cloud print</t>
         </is>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -492,27 +492,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>server1_1761310420.txt</t>
+          <t>server1_1761357206.txt</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>45.135.232.24</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>2025-10-24 22:06:22.958</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>2025-10-24 22:06:23.597</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -522,26 +522,18 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2025-10-24 08:54:33.844
-2025-10-24 08:55:29.784
-2025-10-24 08:56:01.719
-1
-exit</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -552,27 +544,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>server1_1761310753.txt</t>
+          <t>server1_1761357991.txt</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>45.135.232.24</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>2025-10-24 22:32:00.696</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-10-24 09:01:06.376</t>
+          <t>2025-10-24 22:32:01.327</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -582,56 +574,49 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>2025-10-24 09:01:25.154
-2025-10-24 09:01:30.286
-1
-exit</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>server1_1761311382.txt</t>
+          <t>server1_1761359529.txt</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>45.135.232.24</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>2025-10-24 22:57:44.789</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-10-24 09:10:23.754</t>
+          <t>2025-10-24 22:57:45.415</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -641,55 +626,49 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2025-10-24 09:10:37.552
-2025-10-24 09:12:40.868
-0</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>137</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>server1_1761311568.txt</t>
+          <t>server1_1761361073.txt</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-10-24 09:17:23.776</t>
+          <t>103.149.12.38</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2025-10-24 23:21:44.122</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>557 minutes and 23 seconds</t>
+          <t>2025-10-24 23:21:47.985</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -697,48 +676,72 @@
           <t>server1</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-10-24 09:54:50.744</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>server1_1761314030.txt</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+          <t>server1_1761362515.txt</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:25:30.547</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:25:31.193</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>server1</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -749,7 +752,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>server1_1761314614.txt</t>
+          <t>server1_1761362739.txt</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -759,17 +762,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>45.135.232.24</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>2025-10-24 23:51:11.031</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-10-24 10:04:24.851</t>
+          <t>2025-10-24 23:51:12.085</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -779,36 +782,29 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2025-10-24 10:04:42.822
-2025-10-24 10:06:35.097
-1
-exit</t>
-        </is>
-      </c>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>server1_1761314803.txt</t>
+          <t>server2_1761356704.txt</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -818,70 +814,78 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-10-24 10:08:35.454</t>
+          <t>45.15.226.135</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2025-10-24 21:55:53.175</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>608 minutes and 35 seconds</t>
+          <t>2025-10-24 21:55:56.747</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>server1</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>/ip cloud print</t>
+        </is>
+      </c>
       <c r="J9" t="n">
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>server1_1761316216.txt</t>
+          <t>server2_1761357364.txt</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>10.175.90.186</t>
+          <t>45.135.232.24</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-10-24 10:30:51.682</t>
+          <t>2025-10-24 22:03:19.121</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-10-24 10:30:51.673</t>
+          <t>2025-10-24 22:03:19.834</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>server1</t>
+          <t>server2</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -897,6 +901,842 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>server2_1761357807.txt</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:28:57.140</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:28:57.836</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>server2_1761359345.txt</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:54:41.110</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:54:41.798</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>server2_1761360889.txt</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:22:26.446</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:22:27.136</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>server2_1761362555.txt</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>36.20.126.21</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:44:28.753</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:44:30.197</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>server2_1761363878.txt</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:48:06.407</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:48:07.064</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>server2</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>server3_1761356704.txt</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-10-24 21:51:30.784</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-10-24 21:51:31.528</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>server3</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>server3_1761357099.txt</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:17:08.137</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:17:08.890</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>server3</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>server3_1761358636.txt</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:42:52.077</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:42:52.753</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>server3</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>server3_1761360180.txt</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:09:58.896</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:09:59.560</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>server3</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>server3_1761361807.txt</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:36:15.132</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:36:15.781</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>server3</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>server4_1761356704.txt</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-10-24 21:53:58.163</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-10-24 21:53:58.818</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>server4_1761357246.txt</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:19:35.491</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:19:36.128</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>server4_1761358784.txt</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>66.132.153.140</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:44:12.620</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:44:14.358</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>echo -e "\x6F\x6B"</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>2</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>server4_1761360262.txt</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:45:19.934</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-10-24 22:45:20.604</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>server4_1761360328.txt</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:13:07.414</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:13:08.085</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>server4_1761361996.txt</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>45.135.232.24</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:38:43.024</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-10-24 23:38:43.669</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>server4</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>